<commit_message>
tambah qtypack di product.
</commit_message>
<xml_diff>
--- a/protected/modules/product.xlsx
+++ b/protected/modules/product.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nginx-1.20\html\eui-mifsaka\protected\modules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24264B0B-00A4-4B3C-9398-7931359C8DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="15996" windowHeight="7356"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Material / Service</t>
   </si>
@@ -74,13 +80,16 @@
   </si>
   <si>
     <t>Lead Time</t>
+  </si>
+  <si>
+    <t>QtyPack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -157,6 +166,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -204,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,9 +249,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,6 +301,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -447,32 +493,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:S1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="58.109375" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
-    <col min="7" max="10" width="15.88671875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" style="2" customWidth="1"/>
-    <col min="12" max="14" width="8.88671875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" customWidth="1"/>
-    <col min="17" max="17" width="7.21875" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="58.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="7" max="10" width="15.85546875" style="2" customWidth="1"/>
+    <col min="11" max="12" width="10.42578125" style="2" customWidth="1"/>
+    <col min="13" max="15" width="8.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="41.25" customHeight="1">
+    <row r="1" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -494,8 +540,9 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -530,34 +577,37 @@
         <v>19</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:T1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.8" footer="0.8"/>
   <pageSetup orientation="portrait"/>

</xml_diff>